<commit_message>
Monday evening report work in library
</commit_message>
<xml_diff>
--- a/r/data/raw/PlantResults_Cu.MIC.xlsx
+++ b/r/data/raw/PlantResults_Cu.MIC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f14c0c83aeaa8c8/Documents/Uni/2025/Session 1/Placements_FOSE7901/Placement 1/Deliverables/r/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f14c0c83aeaa8c8/Documents/Uni/2025/Session 1/Placements_FOSE7901/Placement 1/Deliverables/r/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="8_{4C056574-35CD-4693-9297-BE17D6D654C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63EB4476-9A93-4C07-9438-0419528B0904}"/>
+  <xr:revisionPtr revIDLastSave="409" documentId="8_{4C056574-35CD-4693-9297-BE17D6D654C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8F455E9-2810-40EE-970F-142C7B449FE2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5A1AF001-11BA-4DFA-9937-B5448583DDE0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{5A1AF001-11BA-4DFA-9937-B5448583DDE0}"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="L.rectus nodules" sheetId="1" r:id="rId4"/>
     <sheet name="L.rectus weights" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="111">
   <si>
     <t>No. of Nodules</t>
   </si>
@@ -644,6 +644,9 @@
   </si>
   <si>
     <t>*adjusted to 1 for analysis (limit of detection)</t>
+  </si>
+  <si>
+    <t>%nod/bump</t>
   </si>
 </sst>
 </file>
@@ -3673,7 +3676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E8A539-EC0A-4222-BB1B-C46D981F76A6}">
   <dimension ref="B1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
@@ -4187,10 +4190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07773AA7-4135-4F1C-80D4-4CEE87E12F0A}">
-  <dimension ref="B1:L22"/>
+  <dimension ref="B1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4632,6 +4635,23 @@
       <c r="F22">
         <f>AVERAGE(L10:L11,L13:L15)</f>
         <v>3.2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24">
+        <f ca="1">100*5/9</f>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="E24">
+        <f ca="1">E20</f>
+        <v>44.444444444444443</v>
+      </c>
+      <c r="F24">
+        <f ca="1">100*8/9</f>
+        <v>88.888888888888886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>